<commit_message>
Atualização do arquivo excel.
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF71AB60-81EB-E341-8FE7-99BF36C8A8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89898FEB-803A-CD4B-AFF6-E4F6ABD5D9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -93,7 +93,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,7 +411,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,7 +442,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44283</v>
+        <v>44648</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44284</v>
+        <v>44649</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44285</v>
+        <v>44650</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44286</v>
+        <v>44651</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44287</v>
+        <v>44652</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44288</v>
+        <v>44653</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44289</v>
+        <v>44654</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44290</v>
+        <v>44655</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44291</v>
+        <v>44656</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -622,7 +622,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44292</v>
+        <v>44657</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44293</v>
+        <v>44658</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>44294</v>
+        <v>44659</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>44295</v>
+        <v>44660</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>44296</v>
+        <v>44661</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>44297</v>
+        <v>44662</v>
       </c>
       <c r="B16">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de casos/óbitos com dados de 12/04.
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89898FEB-803A-CD4B-AFF6-E4F6ABD5D9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6845F45-C16F-7F4C-BB19-A1BF81B478C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,6 +740,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>44663</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>326803</v>
+      </c>
+      <c r="D17">
+        <v>6337</v>
+      </c>
+      <c r="E17">
+        <v>29</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização com dados até 13/04.
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6845F45-C16F-7F4C-BB19-A1BF81B478C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CCECE9-5402-524C-9AC4-81F231E0A2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,6 +760,26 @@
         <v>2</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>44664</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>326834</v>
+      </c>
+      <c r="D18">
+        <v>6338</v>
+      </c>
+      <c r="E18">
+        <v>31</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de casos/óbitos até 22/04/22
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CCECE9-5402-524C-9AC4-81F231E0A2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A18931-C8B2-ED45-818A-E880A56BDA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,6 +780,186 @@
         <v>1</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>44665</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>326862</v>
+      </c>
+      <c r="D19">
+        <v>6338</v>
+      </c>
+      <c r="E19">
+        <v>28</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>44666</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>326879</v>
+      </c>
+      <c r="D20">
+        <v>6339</v>
+      </c>
+      <c r="E20">
+        <v>17</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>44667</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>326894</v>
+      </c>
+      <c r="D21">
+        <v>6339</v>
+      </c>
+      <c r="E21">
+        <v>15</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>44668</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>326902</v>
+      </c>
+      <c r="D22">
+        <v>6339</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>44669</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>326909</v>
+      </c>
+      <c r="D23">
+        <v>6339</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>44670</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>326928</v>
+      </c>
+      <c r="D24">
+        <v>6340</v>
+      </c>
+      <c r="E24">
+        <v>19</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>44671</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>326949</v>
+      </c>
+      <c r="D25">
+        <v>6341</v>
+      </c>
+      <c r="E25">
+        <v>21</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>44672</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>326970</v>
+      </c>
+      <c r="D26">
+        <v>6341</v>
+      </c>
+      <c r="E26">
+        <v>21</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>44673</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>326989</v>
+      </c>
+      <c r="D27">
+        <v>6342</v>
+      </c>
+      <c r="E27">
+        <v>19</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Dados de casos/óbitos até 26/04/22
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A18931-C8B2-ED45-818A-E880A56BDA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820F24C3-9FD3-8646-B1EE-2C1EF3CB2155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -960,6 +960,86 @@
         <v>1</v>
       </c>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>44674</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>327005</v>
+      </c>
+      <c r="D28">
+        <v>6342</v>
+      </c>
+      <c r="E28">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>44675</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>327016</v>
+      </c>
+      <c r="D29">
+        <v>6342</v>
+      </c>
+      <c r="E29">
+        <v>11</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>44676</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>327026</v>
+      </c>
+      <c r="D30">
+        <v>6342</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>44677</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>327037</v>
+      </c>
+      <c r="D31">
+        <v>6342</v>
+      </c>
+      <c r="E31">
+        <v>11</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de casos/óbitos até 30/04/22
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820F24C3-9FD3-8646-B1EE-2C1EF3CB2155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC350DD-AB22-0F46-99BE-4A6C91DB0236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1040,6 +1040,86 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>44678</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>327052</v>
+      </c>
+      <c r="D32">
+        <v>6342</v>
+      </c>
+      <c r="E32">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>44679</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>327065</v>
+      </c>
+      <c r="D33">
+        <v>6342</v>
+      </c>
+      <c r="E33">
+        <v>13</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>44680</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>327071</v>
+      </c>
+      <c r="D34">
+        <v>6343</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>44681</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>327076</v>
+      </c>
+      <c r="D35">
+        <v>6343</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de casos/óbitos até o dia 13/05/22
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC350DD-AB22-0F46-99BE-4A6C91DB0236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD0AE15-4FB9-1749-A2BB-659E044ED8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1120,6 +1120,266 @@
         <v>0</v>
       </c>
     </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>327081</v>
+      </c>
+      <c r="D36">
+        <v>6343</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>44683</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>327089</v>
+      </c>
+      <c r="D37">
+        <v>6343</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>327099</v>
+      </c>
+      <c r="D38">
+        <v>6344</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>44685</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>327106</v>
+      </c>
+      <c r="D39">
+        <v>6344</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>327114</v>
+      </c>
+      <c r="D40">
+        <v>6344</v>
+      </c>
+      <c r="E40">
+        <v>13</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>327132</v>
+      </c>
+      <c r="D41">
+        <v>6344</v>
+      </c>
+      <c r="E41">
+        <v>18</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>327144</v>
+      </c>
+      <c r="D42">
+        <v>6344</v>
+      </c>
+      <c r="E42">
+        <v>12</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>327157</v>
+      </c>
+      <c r="D43">
+        <v>6344</v>
+      </c>
+      <c r="E43">
+        <v>13</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>327167</v>
+      </c>
+      <c r="D44">
+        <v>6345</v>
+      </c>
+      <c r="E44">
+        <v>10</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>327179</v>
+      </c>
+      <c r="D45">
+        <v>6345</v>
+      </c>
+      <c r="E45">
+        <v>12</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>327198</v>
+      </c>
+      <c r="D46">
+        <v>6345</v>
+      </c>
+      <c r="E46">
+        <v>19</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>44693</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>327218</v>
+      </c>
+      <c r="D47">
+        <v>6345</v>
+      </c>
+      <c r="E47">
+        <v>20</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>44694</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>327238</v>
+      </c>
+      <c r="D48">
+        <v>6345</v>
+      </c>
+      <c r="E48">
+        <v>20</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de casos/óbitos até 25/05/22
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD0AE15-4FB9-1749-A2BB-659E044ED8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904E1971-AD3C-3446-B0FC-A54AE0E846BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1380,6 +1380,246 @@
         <v>0</v>
       </c>
     </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>44695</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>327254</v>
+      </c>
+      <c r="D49">
+        <v>6345</v>
+      </c>
+      <c r="E49">
+        <v>16</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>44696</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>327271</v>
+      </c>
+      <c r="D50">
+        <v>6345</v>
+      </c>
+      <c r="E50">
+        <v>17</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>44697</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>327284</v>
+      </c>
+      <c r="D51">
+        <v>6345</v>
+      </c>
+      <c r="E51">
+        <v>13</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>44698</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>327298</v>
+      </c>
+      <c r="D52">
+        <v>6346</v>
+      </c>
+      <c r="E52">
+        <v>14</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>44699</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>327314</v>
+      </c>
+      <c r="D53">
+        <v>6346</v>
+      </c>
+      <c r="E53">
+        <v>16</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>44700</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>327335</v>
+      </c>
+      <c r="D54">
+        <v>6346</v>
+      </c>
+      <c r="E54">
+        <v>21</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>44701</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>327349</v>
+      </c>
+      <c r="D55">
+        <v>6346</v>
+      </c>
+      <c r="E55">
+        <v>14</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>44702</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>327363</v>
+      </c>
+      <c r="D56">
+        <v>6346</v>
+      </c>
+      <c r="E56">
+        <v>14</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>44703</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>327373</v>
+      </c>
+      <c r="D57">
+        <v>6346</v>
+      </c>
+      <c r="E57">
+        <v>10</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>327379</v>
+      </c>
+      <c r="D58">
+        <v>6346</v>
+      </c>
+      <c r="E58">
+        <v>6</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>327397</v>
+      </c>
+      <c r="D59">
+        <v>6347</v>
+      </c>
+      <c r="E59">
+        <v>18</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>327411</v>
+      </c>
+      <c r="D60">
+        <v>6347</v>
+      </c>
+      <c r="E60">
+        <v>14</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de casos/óbitos até 26/05/22
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904E1971-AD3C-3446-B0FC-A54AE0E846BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7804B95-69A4-2948-9E5F-C02F7394BD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1620,6 +1620,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>44707</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>327417</v>
+      </c>
+      <c r="D61">
+        <f>D60+F60</f>
+        <v>6347</v>
+      </c>
+      <c r="E61">
+        <v>8</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>327429</v>
+      </c>
+      <c r="D62">
+        <v>6347</v>
+      </c>
+      <c r="E62">
+        <v>12</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de casos/óbitos até 30/05/22.
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7804B95-69A4-2948-9E5F-C02F7394BD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C4CCFF-3215-8E4A-9825-C0080E04BF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1661,6 +1661,66 @@
         <v>0</v>
       </c>
     </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>44709</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>327439</v>
+      </c>
+      <c r="D63">
+        <v>6348</v>
+      </c>
+      <c r="E63">
+        <v>10</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>44710</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>327442</v>
+      </c>
+      <c r="D64">
+        <v>6348</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>44711</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>327451</v>
+      </c>
+      <c r="D65">
+        <v>6348</v>
+      </c>
+      <c r="E65">
+        <v>9</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de casos/óbitos até 28/06/22
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C4CCFF-3215-8E4A-9825-C0080E04BF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA6480E-F029-EC4F-BFF7-3B71049F1162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1721,6 +1721,466 @@
         <v>0</v>
       </c>
     </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>327458</v>
+      </c>
+      <c r="D66">
+        <v>6348</v>
+      </c>
+      <c r="E66">
+        <v>7</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>327474</v>
+      </c>
+      <c r="D67">
+        <v>6348</v>
+      </c>
+      <c r="E67">
+        <v>16</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>327490</v>
+      </c>
+      <c r="D68">
+        <v>6348</v>
+      </c>
+      <c r="E68">
+        <v>16</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>327517</v>
+      </c>
+      <c r="D69">
+        <v>6348</v>
+      </c>
+      <c r="E69">
+        <v>27</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>44716</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>327528</v>
+      </c>
+      <c r="D70">
+        <v>6348</v>
+      </c>
+      <c r="E70">
+        <v>11</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>44717</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>327538</v>
+      </c>
+      <c r="D71">
+        <v>6348</v>
+      </c>
+      <c r="E71">
+        <v>10</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>327552</v>
+      </c>
+      <c r="D72">
+        <v>6348</v>
+      </c>
+      <c r="E72">
+        <v>14</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>327574</v>
+      </c>
+      <c r="D73">
+        <v>6348</v>
+      </c>
+      <c r="E73">
+        <v>22</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>327597</v>
+      </c>
+      <c r="D74">
+        <v>6349</v>
+      </c>
+      <c r="E74">
+        <v>23</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>327638</v>
+      </c>
+      <c r="D75">
+        <v>6349</v>
+      </c>
+      <c r="E75">
+        <v>41</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>44722</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>327687</v>
+      </c>
+      <c r="D76">
+        <v>6350</v>
+      </c>
+      <c r="E76">
+        <v>49</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>327737</v>
+      </c>
+      <c r="D77">
+        <v>6351</v>
+      </c>
+      <c r="E77">
+        <v>15</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>44726</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>327777</v>
+      </c>
+      <c r="D78">
+        <v>6352</v>
+      </c>
+      <c r="E78">
+        <v>40</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>44727</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>327910</v>
+      </c>
+      <c r="D79">
+        <v>6353</v>
+      </c>
+      <c r="E79">
+        <v>133</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>327993</v>
+      </c>
+      <c r="D80">
+        <v>6353</v>
+      </c>
+      <c r="E80">
+        <v>83</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>44729</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>328042</v>
+      </c>
+      <c r="D81">
+        <v>6353</v>
+      </c>
+      <c r="E81">
+        <v>49</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>44732</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>328119</v>
+      </c>
+      <c r="D82">
+        <v>6353</v>
+      </c>
+      <c r="E82">
+        <v>23</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>44733</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>328260</v>
+      </c>
+      <c r="D83">
+        <v>6354</v>
+      </c>
+      <c r="E83">
+        <v>141</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>44734</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>328561</v>
+      </c>
+      <c r="D84">
+        <v>6354</v>
+      </c>
+      <c r="E84">
+        <v>301</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>44735</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>328744</v>
+      </c>
+      <c r="D85">
+        <v>6355</v>
+      </c>
+      <c r="E85">
+        <v>183</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>44736</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>328955</v>
+      </c>
+      <c r="D86">
+        <v>6355</v>
+      </c>
+      <c r="E86">
+        <v>211</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>44739</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>329405</v>
+      </c>
+      <c r="D87">
+        <v>6356</v>
+      </c>
+      <c r="E87">
+        <v>114</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>44740</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>329686</v>
+      </c>
+      <c r="D88">
+        <v>6357</v>
+      </c>
+      <c r="E88">
+        <v>282</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de casos/óbitos com dados do dia 29/06/22
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA6480E-F029-EC4F-BFF7-3B71049F1162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6A86EA-98DD-A34F-8D80-99EBA28E8C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+      <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2181,6 +2181,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>44741</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>330074</v>
+      </c>
+      <c r="D89">
+        <v>6358</v>
+      </c>
+      <c r="E89">
+        <v>388</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização com dados de casos/óbitos de 30/06/22
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6A86EA-98DD-A34F-8D80-99EBA28E8C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE37C66-D0D3-6F43-9C8B-F533870F95CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2201,6 +2201,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>44742</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>330327</v>
+      </c>
+      <c r="D90">
+        <v>6358</v>
+      </c>
+      <c r="E90">
+        <v>253</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de casos/óbitos até dia 08/07/22
</commit_message>
<xml_diff>
--- a/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
+++ b/br-se-covid19-casos-obitos/input/casos_obitos_sergipe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/dadosabertossergipe/covid19/br-se-covid19-casos-obitos/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE37C66-D0D3-6F43-9C8B-F533870F95CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC1F934-D3C5-2F4F-8315-6C395A1F96AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="26740" windowHeight="13400" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
+    <workbookView xWindow="27320" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{E21C5369-0FE3-0A48-82AA-E24CCCB2F14B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9C9ECB-EE57-9143-A29C-BA511C905A26}">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2221,6 +2221,106 @@
         <v>0</v>
       </c>
     </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>44746</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>331286</v>
+      </c>
+      <c r="D91">
+        <v>6360</v>
+      </c>
+      <c r="E91">
+        <v>83</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>44747</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>331729</v>
+      </c>
+      <c r="D92">
+        <v>6361</v>
+      </c>
+      <c r="E92">
+        <v>443</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>44748</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>332454</v>
+      </c>
+      <c r="D93">
+        <v>6363</v>
+      </c>
+      <c r="E93">
+        <v>725</v>
+      </c>
+      <c r="F93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>44749</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>332978</v>
+      </c>
+      <c r="D94">
+        <v>6364</v>
+      </c>
+      <c r="E94">
+        <v>524</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>44750</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>333606</v>
+      </c>
+      <c r="D95">
+        <v>6366</v>
+      </c>
+      <c r="E95">
+        <v>628</v>
+      </c>
+      <c r="F95">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>